<commit_message>
Unit tests + backlog
</commit_message>
<xml_diff>
--- a/Sprint Backlog/SprintBacklog.xlsx
+++ b/Sprint Backlog/SprintBacklog.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="75">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1467,7 +1467,7 @@
         <v>72</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>6</v>
@@ -1488,7 +1488,10 @@
         <v>2</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -2438,8 +2441,11 @@
       <c r="B45">
         <v>6</v>
       </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
       <c r="D45" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E45">
         <v>6</v>
@@ -2458,6 +2464,12 @@
       </c>
       <c r="J45">
         <v>6</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -2543,9 +2555,6 @@
       <c r="B48">
         <v>2</v>
       </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
       <c r="D48" s="4" t="s">
         <v>23</v>
       </c>
@@ -2565,6 +2574,9 @@
         <v>2</v>
       </c>
       <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
         <v>2</v>
       </c>
     </row>
@@ -2575,9 +2587,6 @@
       <c r="B49">
         <v>6</v>
       </c>
-      <c r="C49">
-        <v>6</v>
-      </c>
       <c r="D49" s="4" t="s">
         <v>23</v>
       </c>
@@ -2597,6 +2606,9 @@
         <v>6</v>
       </c>
       <c r="J49">
+        <v>6</v>
+      </c>
+      <c r="K49">
         <v>6</v>
       </c>
     </row>

</xml_diff>